<commit_message>
Update weights and eggs
</commit_message>
<xml_diff>
--- a/data/raw/weights.xlsx
+++ b/data/raw/weights.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hab737\GitHub\personal-goals\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harvey\Github\personal-goals\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E400822-1991-4858-AB08-7AD79FE267BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81015AB5-E860-42FE-8B28-EDE9D1D872C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15885" xr2:uid="{6673F513-5FF6-4B04-9025-EC09F1BEA076}"/>
+    <workbookView xWindow="369" yWindow="2897" windowWidth="21780" windowHeight="14700" xr2:uid="{6673F513-5FF6-4B04-9025-EC09F1BEA076}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -391,18 +391,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947E12DA-C847-475D-917E-A98794A15607}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -410,7 +410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>44216</v>
       </c>
@@ -421,7 +421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>44217</v>
       </c>
@@ -432,7 +432,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>44218</v>
       </c>
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>44219</v>
       </c>
@@ -454,7 +454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>44220</v>
       </c>
@@ -465,7 +465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>44221</v>
       </c>
@@ -476,7 +476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>44222</v>
       </c>
@@ -485,6 +485,83 @@
       </c>
       <c r="C8">
         <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="1">
+        <v>44223</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="1">
+        <v>44224</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="1">
+        <v>44225</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="1">
+        <v>44226</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" s="1">
+        <v>44227</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" s="1">
+        <v>44229</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update eggs and weights
</commit_message>
<xml_diff>
--- a/data/raw/weights.xlsx
+++ b/data/raw/weights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harvey\Github\personal-goals\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81015AB5-E860-42FE-8B28-EDE9D1D872C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6366CE68-4FFA-4510-A9B5-0CE702EE0E7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="369" yWindow="2897" windowWidth="21780" windowHeight="14700" xr2:uid="{6673F513-5FF6-4B04-9025-EC09F1BEA076}"/>
+    <workbookView xWindow="26" yWindow="2554" windowWidth="21780" windowHeight="14700" xr2:uid="{6673F513-5FF6-4B04-9025-EC09F1BEA076}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947E12DA-C847-475D-917E-A98794A15607}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -564,6 +564,39 @@
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" s="1">
+        <v>44230</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" s="1">
+        <v>44231</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" s="1">
+        <v>44232</v>
+      </c>
+      <c r="B18">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating eggs and weights
</commit_message>
<xml_diff>
--- a/data/raw/weights.xlsx
+++ b/data/raw/weights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hab737\GitHub\personal-goals\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harvey\Github\personal-goals\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30E5190-BAF5-4248-B80E-1FC0AD605EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D619D01-4B01-4108-8A4D-A33238E2BE14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3810" windowWidth="28800" windowHeight="15885" xr2:uid="{6673F513-5FF6-4B04-9025-EC09F1BEA076}"/>
+    <workbookView xWindow="63960" yWindow="-870" windowWidth="24690" windowHeight="15930" xr2:uid="{6673F513-5FF6-4B04-9025-EC09F1BEA076}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>chinups</t>
   </si>
   <si>
     <t>pushups</t>
+  </si>
+  <si>
+    <t>v-crunch</t>
+  </si>
+  <si>
+    <t>penguins</t>
+  </si>
+  <si>
+    <t>shrugs</t>
   </si>
 </sst>
 </file>
@@ -391,26 +400,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947E12DA-C847-475D-917E-A98794A15607}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>44216</v>
       </c>
@@ -420,8 +438,17 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>44217</v>
       </c>
@@ -431,8 +458,17 @@
       <c r="C3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>44218</v>
       </c>
@@ -442,8 +478,17 @@
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>44219</v>
       </c>
@@ -453,8 +498,17 @@
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>44220</v>
       </c>
@@ -464,8 +518,17 @@
       <c r="C6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>44221</v>
       </c>
@@ -475,8 +538,17 @@
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>44222</v>
       </c>
@@ -486,8 +558,17 @@
       <c r="C8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>44223</v>
       </c>
@@ -497,8 +578,17 @@
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>44224</v>
       </c>
@@ -508,8 +598,17 @@
       <c r="C10">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>44225</v>
       </c>
@@ -519,8 +618,17 @@
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>44226</v>
       </c>
@@ -530,8 +638,17 @@
       <c r="C12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>44227</v>
       </c>
@@ -541,8 +658,17 @@
       <c r="C13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>44228</v>
       </c>
@@ -552,8 +678,17 @@
       <c r="C14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>44229</v>
       </c>
@@ -563,8 +698,17 @@
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>44230</v>
       </c>
@@ -574,8 +718,17 @@
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>44231</v>
       </c>
@@ -585,8 +738,17 @@
       <c r="C17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>44232</v>
       </c>
@@ -596,8 +758,17 @@
       <c r="C18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>44233</v>
       </c>
@@ -607,8 +778,17 @@
       <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>44234</v>
       </c>
@@ -618,8 +798,17 @@
       <c r="C20">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>44235</v>
       </c>
@@ -629,8 +818,17 @@
       <c r="C21">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>44236</v>
       </c>
@@ -640,8 +838,17 @@
       <c r="C22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>44237</v>
       </c>
@@ -651,8 +858,17 @@
       <c r="C23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>44238</v>
       </c>
@@ -662,8 +878,17 @@
       <c r="C24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>44239</v>
       </c>
@@ -672,6 +897,35 @@
       </c>
       <c r="C25">
         <v>45</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A26" s="1">
+        <v>44240</v>
+      </c>
+      <c r="B26">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>40</v>
+      </c>
+      <c r="E26">
+        <v>35</v>
+      </c>
+      <c r="F26">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>